<commit_message>
agregue nuevas hoja a al excel de perú, informacion de las personas de ese pais
</commit_message>
<xml_diff>
--- a/Niveles/analisis_cargos_peru.xlsx
+++ b/Niveles/analisis_cargos_peru.xlsx
@@ -5,25 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gpavez\Desktop\Compensaciones\git\compensaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gpavez\Desktop\Compensaciones\git\compensaciones\Niveles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="7245" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos_Originales" sheetId="1" r:id="rId1"/>
     <sheet name="Analisis_Por_Cargo" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Analisis_Por_Cargo!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Hoja1!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="201">
   <si>
     <t>DNI</t>
   </si>
@@ -191,6 +193,441 @@
   </si>
   <si>
     <t>Nivel_Gabriel</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Jefatura</t>
+  </si>
+  <si>
+    <t>Victor Manuel Gomez Nuñez</t>
+  </si>
+  <si>
+    <t>07884700</t>
+  </si>
+  <si>
+    <t>Jorge Hermes Heredia Castillo</t>
+  </si>
+  <si>
+    <t>10554111</t>
+  </si>
+  <si>
+    <t>Erick Blass Guzmán Muñante</t>
+  </si>
+  <si>
+    <t>40821076</t>
+  </si>
+  <si>
+    <t>Marianella Isabel Guevara Castilla</t>
+  </si>
+  <si>
+    <t>41532675</t>
+  </si>
+  <si>
+    <t>Patricia Alejandra Cordova Valdivia</t>
+  </si>
+  <si>
+    <t>44392341</t>
+  </si>
+  <si>
+    <t>Karin Elizabeth Jurado Delgado</t>
+  </si>
+  <si>
+    <t>41537579</t>
+  </si>
+  <si>
+    <t>Milagros Herminia Maldonado Frias</t>
+  </si>
+  <si>
+    <t>07967737</t>
+  </si>
+  <si>
+    <t>Xiomara Morales Rivera</t>
+  </si>
+  <si>
+    <t>08163648</t>
+  </si>
+  <si>
+    <t>Nidia Krysle Leyva Reyes</t>
+  </si>
+  <si>
+    <t>42872627</t>
+  </si>
+  <si>
+    <t>Johan Erick Gaspar Vasquez</t>
+  </si>
+  <si>
+    <t>44261568</t>
+  </si>
+  <si>
+    <t>Patricia Rocio Flores Mariñas</t>
+  </si>
+  <si>
+    <t>44728906</t>
+  </si>
+  <si>
+    <t>Karen Chirinos Gomez</t>
+  </si>
+  <si>
+    <t>41361370</t>
+  </si>
+  <si>
+    <t>Thais Victoria Priscila Ruiz Perez</t>
+  </si>
+  <si>
+    <t>73760726</t>
+  </si>
+  <si>
+    <t>Gloria Luisa Vera Preciado</t>
+  </si>
+  <si>
+    <t>40028202</t>
+  </si>
+  <si>
+    <t>Fabian Delman Paredes Cabrera</t>
+  </si>
+  <si>
+    <t>40045681</t>
+  </si>
+  <si>
+    <t>Giulianna Carmela Huertas Cansino</t>
+  </si>
+  <si>
+    <t>44259638</t>
+  </si>
+  <si>
+    <t>Carmen Cardenas Uribe</t>
+  </si>
+  <si>
+    <t>45077288</t>
+  </si>
+  <si>
+    <t>Sergio Andre Vargas Tito</t>
+  </si>
+  <si>
+    <t>75706696</t>
+  </si>
+  <si>
+    <t>Kely Keyla Quiroz Cordova</t>
+  </si>
+  <si>
+    <t>47403138</t>
+  </si>
+  <si>
+    <t>Jessica Lizbeth Rodriguez Ruiz</t>
+  </si>
+  <si>
+    <t>41731438</t>
+  </si>
+  <si>
+    <t>Erika Gomez Bazán</t>
+  </si>
+  <si>
+    <t>42628174</t>
+  </si>
+  <si>
+    <t>Liliana Isabel Camarena De La Cruz</t>
+  </si>
+  <si>
+    <t>08165431</t>
+  </si>
+  <si>
+    <t>David Randolf Amado Santiago</t>
+  </si>
+  <si>
+    <t>46768320</t>
+  </si>
+  <si>
+    <t>Miguel Angel Cacsire Saboya</t>
+  </si>
+  <si>
+    <t>42330129</t>
+  </si>
+  <si>
+    <t>Virginia Veronica Llanos Chilcón</t>
+  </si>
+  <si>
+    <t>46469135</t>
+  </si>
+  <si>
+    <t>Yesenia Nathalie Díaz Zelada</t>
+  </si>
+  <si>
+    <t>46687380</t>
+  </si>
+  <si>
+    <t>Yuleidy Karina Matos Ruiz</t>
+  </si>
+  <si>
+    <t>49020832</t>
+  </si>
+  <si>
+    <t>Pedro Diego Torres Huarcaya</t>
+  </si>
+  <si>
+    <t>75129386</t>
+  </si>
+  <si>
+    <t>Laura Stefany Velasquez Quispe</t>
+  </si>
+  <si>
+    <t>72852358</t>
+  </si>
+  <si>
+    <t>Erik Martin Schultz Carreño</t>
+  </si>
+  <si>
+    <t>09960373</t>
+  </si>
+  <si>
+    <t>Carlini Alberto Ortiz Meza</t>
+  </si>
+  <si>
+    <t>75723740</t>
+  </si>
+  <si>
+    <t>Claudia Victoria Novoa Reyes</t>
+  </si>
+  <si>
+    <t>42096614</t>
+  </si>
+  <si>
+    <t>Carmen Luisa Calisaya Huaman</t>
+  </si>
+  <si>
+    <t>10745998</t>
+  </si>
+  <si>
+    <t>Roxana Avalos Chacchi</t>
+  </si>
+  <si>
+    <t>70338253</t>
+  </si>
+  <si>
+    <t>Elly Noriko Moromizato Tomita</t>
+  </si>
+  <si>
+    <t>73007608</t>
+  </si>
+  <si>
+    <t>Karla Milagros Reusche Gianotti</t>
+  </si>
+  <si>
+    <t>45457395</t>
+  </si>
+  <si>
+    <t>Oscar David Reyes Mamani</t>
+  </si>
+  <si>
+    <t>47096248</t>
+  </si>
+  <si>
+    <t>Lenin Riva Lopez</t>
+  </si>
+  <si>
+    <t>74318067</t>
+  </si>
+  <si>
+    <t>Susan Lys Rodriguez Flores</t>
+  </si>
+  <si>
+    <t>45197954</t>
+  </si>
+  <si>
+    <t>Dayanna Katherine Sanchez Campos</t>
+  </si>
+  <si>
+    <t>70819004</t>
+  </si>
+  <si>
+    <t>Franco Vargas Elera</t>
+  </si>
+  <si>
+    <t>41239663</t>
+  </si>
+  <si>
+    <t>Brenda Xiomara Chauca Juro</t>
+  </si>
+  <si>
+    <t>71036317</t>
+  </si>
+  <si>
+    <t>Christopher Andy Rios Rojas</t>
+  </si>
+  <si>
+    <t>72643279</t>
+  </si>
+  <si>
+    <t>Guadalupe Elizabeth Mantilla Apolinario</t>
+  </si>
+  <si>
+    <t>74071527</t>
+  </si>
+  <si>
+    <t>Maria Cristina Magallanes Chauca</t>
+  </si>
+  <si>
+    <t>72379762</t>
+  </si>
+  <si>
+    <t>Ericka Vanessa Sullca Pozo</t>
+  </si>
+  <si>
+    <t>48570683</t>
+  </si>
+  <si>
+    <t>Diana Madelen Ordoñez Chamorro</t>
+  </si>
+  <si>
+    <t>72508217</t>
+  </si>
+  <si>
+    <t>Luis Jonathan Diaz Yaringaño</t>
+  </si>
+  <si>
+    <t>41872223</t>
+  </si>
+  <si>
+    <t>Nancy Fabiola Satudio Leon</t>
+  </si>
+  <si>
+    <t>70396121</t>
+  </si>
+  <si>
+    <t>Angela Melissa Faustino Oropeza</t>
+  </si>
+  <si>
+    <t>75895504</t>
+  </si>
+  <si>
+    <t>Alcira Yolanda Lima Armas</t>
+  </si>
+  <si>
+    <t>09489393</t>
+  </si>
+  <si>
+    <t>Jose Luis Leandro Paucar</t>
+  </si>
+  <si>
+    <t>42348577</t>
+  </si>
+  <si>
+    <t>Marcos Chuchón Rojas</t>
+  </si>
+  <si>
+    <t>77292189</t>
+  </si>
+  <si>
+    <t>Waldo Aponte Valderrama</t>
+  </si>
+  <si>
+    <t>46564941</t>
+  </si>
+  <si>
+    <t>Jhair Manuel Cuya Curo</t>
+  </si>
+  <si>
+    <t>70466176</t>
+  </si>
+  <si>
+    <t>Virginia Romero Paredes</t>
+  </si>
+  <si>
+    <t>41541700</t>
+  </si>
+  <si>
+    <t>Diego Arturo Gutierrez Descalzi</t>
+  </si>
+  <si>
+    <t>44727952</t>
+  </si>
+  <si>
+    <t>Angel Gabriel Ordoñez Cataño</t>
+  </si>
+  <si>
+    <t>75124299</t>
+  </si>
+  <si>
+    <t>Cristian Omar Tapayuri Quispe</t>
+  </si>
+  <si>
+    <t>43121436</t>
+  </si>
+  <si>
+    <t>Raquel Retamozo Utani</t>
+  </si>
+  <si>
+    <t>75468069</t>
+  </si>
+  <si>
+    <t>Yohanna Antonia Copacondori Puma</t>
+  </si>
+  <si>
+    <t>76930633</t>
+  </si>
+  <si>
+    <t>Jhanet Fiorella Torres Faustino</t>
+  </si>
+  <si>
+    <t>76740804</t>
+  </si>
+  <si>
+    <t>Karen Natali Roque Gonzales</t>
+  </si>
+  <si>
+    <t>70874737</t>
+  </si>
+  <si>
+    <t>Ysabel Abigail Garcia Aroni</t>
+  </si>
+  <si>
+    <t>70894311</t>
+  </si>
+  <si>
+    <t>Fatima Del Pilar Lopez Apaza</t>
+  </si>
+  <si>
+    <t>75359379</t>
+  </si>
+  <si>
+    <t>Nolberto Geremy Aburto Avila</t>
+  </si>
+  <si>
+    <t>75869849</t>
+  </si>
+  <si>
+    <t>Osmar Enrique Diaz Ramos</t>
+  </si>
+  <si>
+    <t>70976536</t>
+  </si>
+  <si>
+    <t>Gerardo Miguel Sanchez Tremel</t>
+  </si>
+  <si>
+    <t>60898190</t>
+  </si>
+  <si>
+    <t>Leonardo Luis Rodriguez Pizarro</t>
+  </si>
+  <si>
+    <t>75485753</t>
+  </si>
+  <si>
+    <t>Joel Armando Torres Cornejo</t>
+  </si>
+  <si>
+    <t>76548442</t>
+  </si>
+  <si>
+    <t>David Chuchon Rojas</t>
+  </si>
+  <si>
+    <t>72699192</t>
   </si>
 </sst>
 </file>
@@ -200,7 +637,7 @@
   <numFmts count="1">
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,16 +657,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -263,12 +725,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -286,10 +801,27 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1621,7 +2153,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,22 +2306,22 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="7">
         <v>2</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="9">
         <v>1550</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="9">
         <v>4600</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="9">
         <v>3075</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="9">
         <v>3075</v>
       </c>
       <c r="G7" s="5">
@@ -1797,22 +2329,22 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="7">
         <v>2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="9">
         <v>1600</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="9">
         <v>2160</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="9">
         <v>1880</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="9">
         <v>1880</v>
       </c>
     </row>
@@ -2457,42 +2989,42 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="8">
         <v>1</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="10">
         <v>12650</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="10">
         <v>12650</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="10">
         <v>12650</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="10">
         <v>12650</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="8">
         <v>1</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="10">
         <v>13530</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="10">
         <v>13530</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="10">
         <v>13530</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="10">
         <v>13530</v>
       </c>
     </row>
@@ -2604,4 +3136,1689 @@
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="15">
+        <v>25</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15">
+        <v>1500</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="15">
+        <v>23.3</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1300</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="17">
+        <v>28.5</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="17">
+        <v>2800</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="17">
+        <v>21.4</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="17">
+        <v>1550</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="15">
+        <v>24.4</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="15">
+        <v>1300</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="17">
+        <v>32.5</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="17">
+        <v>3200</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="17">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="F8" s="17">
+        <v>3200</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="21">
+        <v>30.5</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="F9" s="21">
+        <v>2800</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="20">
+        <v>23.4</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="20">
+        <v>2300</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="17">
+        <v>23</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="F11" s="17">
+        <v>1300</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="17">
+        <v>28.2</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="F12" s="17">
+        <v>1300</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="15">
+        <v>29.9</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="F13" s="15">
+        <v>3300</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="15">
+        <v>25.9</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="F14" s="15">
+        <v>3200</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="17">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="F15" s="17">
+        <v>1300</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="15">
+        <v>24</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="15">
+        <v>1500</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="17">
+        <v>22.2</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="17">
+        <v>1500</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="15">
+        <v>33</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F18" s="15">
+        <v>2500</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="15">
+        <v>19.2</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="F19" s="15">
+        <v>1250</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="17">
+        <v>30.4</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="F20" s="17">
+        <v>8000</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="17">
+        <v>26.5</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="F21" s="17">
+        <v>2900</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="15">
+        <v>29.4</v>
+      </c>
+      <c r="E22" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="F22" s="15">
+        <v>2700</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="17">
+        <v>49.9</v>
+      </c>
+      <c r="E23" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="F23" s="17">
+        <v>5000</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="17">
+        <v>28.9</v>
+      </c>
+      <c r="E24" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="F24" s="17">
+        <v>1600</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="15">
+        <v>37.9</v>
+      </c>
+      <c r="E25" s="15">
+        <v>1</v>
+      </c>
+      <c r="F25" s="15">
+        <v>1600</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="15">
+        <v>31.9</v>
+      </c>
+      <c r="E26" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F26" s="15">
+        <v>2540</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="17">
+        <v>42.8</v>
+      </c>
+      <c r="E27" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="F27" s="17">
+        <v>1650</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="17">
+        <v>34.5</v>
+      </c>
+      <c r="E28" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="F28" s="17">
+        <v>4000</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="17">
+        <v>23.3</v>
+      </c>
+      <c r="E29" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="F29" s="17">
+        <v>1550</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="17">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="E30" s="17">
+        <v>1.4</v>
+      </c>
+      <c r="F30" s="17">
+        <v>10980</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="15">
+        <v>24.4</v>
+      </c>
+      <c r="E31" s="15">
+        <v>1.4</v>
+      </c>
+      <c r="F31" s="15">
+        <v>1550</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="17">
+        <v>27.9</v>
+      </c>
+      <c r="E32" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="F32" s="17">
+        <v>3080</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="17">
+        <v>31</v>
+      </c>
+      <c r="E33" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="F33" s="17">
+        <v>2700</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="15">
+        <v>30.1</v>
+      </c>
+      <c r="E34" s="15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F34" s="15">
+        <v>3600</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="15">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="E35" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>8500</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="15">
+        <v>40.1</v>
+      </c>
+      <c r="E36" s="15">
+        <v>2.9</v>
+      </c>
+      <c r="F36" s="15">
+        <v>1600</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="17">
+        <v>29.7</v>
+      </c>
+      <c r="E37" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="F37" s="17">
+        <v>3680</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="15">
+        <v>47.4</v>
+      </c>
+      <c r="E38" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="F38" s="15">
+        <v>3250</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="15">
+        <v>44</v>
+      </c>
+      <c r="E39" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="F39" s="15">
+        <v>2900</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="15">
+        <v>36</v>
+      </c>
+      <c r="E40" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="F40" s="15">
+        <v>3810</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="15">
+        <v>25.8</v>
+      </c>
+      <c r="E41" s="15">
+        <v>4</v>
+      </c>
+      <c r="F41" s="15">
+        <v>1830</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="15">
+        <v>35.1</v>
+      </c>
+      <c r="E42" s="15">
+        <v>4.2</v>
+      </c>
+      <c r="F42" s="15">
+        <v>4200</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="17">
+        <v>42.2</v>
+      </c>
+      <c r="E43" s="17">
+        <v>5</v>
+      </c>
+      <c r="F43" s="17">
+        <v>4500</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="17">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E44" s="17">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F44" s="17">
+        <v>1830</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="15">
+        <v>29.9</v>
+      </c>
+      <c r="E45" s="15">
+        <v>5.4</v>
+      </c>
+      <c r="F45" s="15">
+        <v>1710</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="15">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E46" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="F46" s="15">
+        <v>10300</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="15">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="E47" s="15">
+        <v>6.3</v>
+      </c>
+      <c r="F47" s="15">
+        <v>10000</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="17">
+        <v>42.9</v>
+      </c>
+      <c r="E48" s="17">
+        <v>6.3</v>
+      </c>
+      <c r="F48" s="17">
+        <v>2500</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="17">
+        <v>41.8</v>
+      </c>
+      <c r="E49" s="17">
+        <v>7.3</v>
+      </c>
+      <c r="F49" s="17">
+        <v>10180</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="17">
+        <v>42.4</v>
+      </c>
+      <c r="E50" s="17">
+        <v>8.1</v>
+      </c>
+      <c r="F50" s="17">
+        <v>1850</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D51" s="17">
+        <v>41.9</v>
+      </c>
+      <c r="E51" s="17">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F51" s="17">
+        <v>3280</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="17">
+        <v>31.3</v>
+      </c>
+      <c r="E52" s="17">
+        <v>8.5</v>
+      </c>
+      <c r="F52" s="17">
+        <v>2800</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="17">
+        <v>42.7</v>
+      </c>
+      <c r="E53" s="17">
+        <v>9.5</v>
+      </c>
+      <c r="F53" s="17">
+        <v>14800</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="15">
+        <v>38.1</v>
+      </c>
+      <c r="E54" s="15">
+        <v>10.1</v>
+      </c>
+      <c r="F54" s="15">
+        <v>17100</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="15">
+        <v>45.6</v>
+      </c>
+      <c r="E55" s="15">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F55" s="15">
+        <v>22500</v>
+      </c>
+      <c r="G55" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="15">
+        <v>40.9</v>
+      </c>
+      <c r="E56" s="15">
+        <v>10.9</v>
+      </c>
+      <c r="F56" s="15">
+        <v>5010</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="15">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E57" s="15">
+        <v>10.9</v>
+      </c>
+      <c r="F57" s="15">
+        <v>4600</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="15">
+        <v>33.1</v>
+      </c>
+      <c r="E58" s="15">
+        <v>11.1</v>
+      </c>
+      <c r="F58" s="15">
+        <v>6020</v>
+      </c>
+      <c r="G58" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" s="17">
+        <v>42.2</v>
+      </c>
+      <c r="E59" s="17">
+        <v>11.6</v>
+      </c>
+      <c r="F59" s="17">
+        <v>5010</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="19">
+        <v>50.2</v>
+      </c>
+      <c r="E60" s="19">
+        <v>11.9</v>
+      </c>
+      <c r="F60" s="19">
+        <v>13530</v>
+      </c>
+      <c r="G60" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D61" s="15">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E61" s="15">
+        <v>12.4</v>
+      </c>
+      <c r="F61" s="15">
+        <v>2960</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="15">
+        <v>47.1</v>
+      </c>
+      <c r="E62" s="15">
+        <v>13</v>
+      </c>
+      <c r="F62" s="15">
+        <v>9270</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="17">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="E63" s="17">
+        <v>13.3</v>
+      </c>
+      <c r="F63" s="17">
+        <v>8600</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="15">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E64" s="15">
+        <v>13.3</v>
+      </c>
+      <c r="F64" s="15">
+        <v>3110</v>
+      </c>
+      <c r="G64" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D65" s="15">
+        <v>55.1</v>
+      </c>
+      <c r="E65" s="15">
+        <v>13.8</v>
+      </c>
+      <c r="F65" s="15">
+        <v>2160</v>
+      </c>
+      <c r="G65" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="19">
+        <v>40.4</v>
+      </c>
+      <c r="E66" s="19">
+        <v>14.5</v>
+      </c>
+      <c r="F66" s="19">
+        <v>12650</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" s="17">
+        <v>49.5</v>
+      </c>
+      <c r="E67" s="17">
+        <v>15.7</v>
+      </c>
+      <c r="F67" s="17">
+        <v>3520</v>
+      </c>
+      <c r="G67" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="17">
+        <v>42.7</v>
+      </c>
+      <c r="E68" s="17">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="F68" s="17">
+        <v>20000</v>
+      </c>
+      <c r="G68" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="17">
+        <v>46.6</v>
+      </c>
+      <c r="E69" s="17">
+        <v>18.7</v>
+      </c>
+      <c r="F69" s="17">
+        <v>9800</v>
+      </c>
+      <c r="G69" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="17">
+        <v>48.8</v>
+      </c>
+      <c r="E70" s="17">
+        <v>22.6</v>
+      </c>
+      <c r="F70" s="17">
+        <v>30000</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="15">
+        <v>58.9</v>
+      </c>
+      <c r="E71" s="15">
+        <v>25.2</v>
+      </c>
+      <c r="F71" s="15">
+        <v>50990</v>
+      </c>
+      <c r="G71" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" s="15">
+        <v>57.3</v>
+      </c>
+      <c r="E72" s="15">
+        <v>25.2</v>
+      </c>
+      <c r="F72" s="15">
+        <v>14750</v>
+      </c>
+      <c r="G72" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G1">
+    <sortState ref="A2:G72">
+      <sortCondition ref="E1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>